<commit_message>
add schema and artifacts from modeling session
</commit_message>
<xml_diff>
--- a/project/excel/linkml_tutorial_2024.xlsx
+++ b/project/excel/linkml_tutorial_2024.xlsx
@@ -7,9 +7,10 @@
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="NamedThing" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Person" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="PersonCollection" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="SampleCollection" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sample" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Air Sample" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Soil Sample" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -415,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -431,12 +432,7 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>description</t>
+          <t>samples</t>
         </is>
       </c>
     </row>
@@ -451,7 +447,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G1"/>
+  <dimension ref="A1:E1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -462,44 +458,37 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>primary_email</t>
+          <t>id</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>birth_date</t>
+          <t>latitude</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>age_in_years</t>
+          <t>longitude</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>vital_status</t>
+          <t>species</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>description</t>
+          <t>sample biome</t>
         </is>
       </c>
     </row>
   </sheetData>
-  <dataValidations count="1">
+  <dataValidations count="2">
     <dataValidation sqref="D2:D1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
-      <formula1>"ALIVE,DEAD,UNKNOWN"</formula1>
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"forest,lake,ocean,desert,air"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -512,7 +501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -523,11 +512,103 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>entries</t>
+          <t>altitude</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>latitude</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>longitude</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>species</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sample biome</t>
         </is>
       </c>
     </row>
   </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"forest,lake,ocean,desert,air"</formula1>
+    </dataValidation>
+  </dataValidations>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>depth</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>latitude</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>longitude</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>species</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sample biome</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <dataValidations count="2">
+    <dataValidation sqref="E2:E1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>""</formula1>
+    </dataValidation>
+    <dataValidation sqref="F2:F1048576" showDropDown="0" showInputMessage="0" showErrorMessage="0" allowBlank="1" type="list">
+      <formula1>"forest,lake,ocean,desert,air"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding working sample data
</commit_message>
<xml_diff>
--- a/project/excel/linkml_tutorial_2024.xlsx
+++ b/project/excel/linkml_tutorial_2024.xlsx
@@ -9,8 +9,8 @@
   <sheets>
     <sheet name="SampleCollection" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sample" sheetId="2" state="visible" r:id="rId2"/>
-    <sheet name="Air Sample" sheetId="3" state="visible" r:id="rId3"/>
-    <sheet name="Soil Sample" sheetId="4" state="visible" r:id="rId4"/>
+    <sheet name="AirSample" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="SoilSample" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -416,7 +416,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -426,11 +426,6 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
-        <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
         <is>
           <t>samples</t>
         </is>
@@ -447,7 +442,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -478,7 +473,12 @@
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>sample biome</t>
+          <t>sample_biome</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>sample_type</t>
         </is>
       </c>
     </row>
@@ -501,7 +501,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -537,7 +537,12 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>sample biome</t>
+          <t>sample_biome</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sample_type</t>
         </is>
       </c>
     </row>
@@ -560,7 +565,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:G1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -596,7 +601,12 @@
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>sample biome</t>
+          <t>sample_biome</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>sample_type</t>
         </is>
       </c>
     </row>

</xml_diff>